<commit_message>
Fixed singular jacobian exit mechanism.
</commit_message>
<xml_diff>
--- a/cases/ieee14/case14.xlsx
+++ b/cases/ieee14/case14.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/cases/ieee14/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F626FE-AAF8-7A4F-8D3C-F7E57D022729}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17955" activeTab="5"/>
+    <workbookView xWindow="5400" yWindow="13480" windowWidth="17280" windowHeight="11280" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -13,63 +19,58 @@
     <sheet name="Slack" sheetId="4" r:id="rId4"/>
     <sheet name="Shunt" sheetId="5" r:id="rId5"/>
     <sheet name="Line" sheetId="6" r:id="rId6"/>
-    <sheet name="Area" sheetId="7" r:id="rId7"/>
-    <sheet name="GENCLS" sheetId="8" r:id="rId8"/>
-    <sheet name="GENROU" sheetId="9" r:id="rId9"/>
-    <sheet name="TG2" sheetId="10" r:id="rId10"/>
-    <sheet name="TGOV1" sheetId="11" r:id="rId11"/>
-    <sheet name="EXDC2" sheetId="12" r:id="rId12"/>
-    <sheet name="Toggler" sheetId="13" r:id="rId13"/>
+    <sheet name="GENCLS" sheetId="7" r:id="rId7"/>
+    <sheet name="Fault" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="144">
+  <si>
+    <t>idx</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Vn</t>
+  </si>
+  <si>
+    <t>vmax</t>
+  </si>
+  <si>
+    <t>vmin</t>
+  </si>
+  <si>
+    <t>v0</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>xcoord</t>
+  </si>
+  <si>
+    <t>ycoord</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
   <si>
     <t>uid</t>
   </si>
   <si>
-    <t>idx</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Vn</t>
-  </si>
-  <si>
-    <t>vmax</t>
-  </si>
-  <si>
-    <t>vmin</t>
-  </si>
-  <si>
-    <t>v0</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>xcoord</t>
-  </si>
-  <si>
-    <t>ycoord</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>zone</t>
-  </si>
-  <si>
-    <t>owner</t>
-  </si>
-  <si>
     <t>Bus 1     HV</t>
   </si>
   <si>
@@ -124,66 +125,66 @@
     <t>PQ_0</t>
   </si>
   <si>
+    <t>PQ_1</t>
+  </si>
+  <si>
+    <t>PQ_2</t>
+  </si>
+  <si>
+    <t>PQ_3</t>
+  </si>
+  <si>
+    <t>PQ_4</t>
+  </si>
+  <si>
+    <t>PQ_5</t>
+  </si>
+  <si>
+    <t>PQ_6</t>
+  </si>
+  <si>
+    <t>PQ_7</t>
+  </si>
+  <si>
+    <t>PQ_8</t>
+  </si>
+  <si>
+    <t>PQ_9</t>
+  </si>
+  <si>
+    <t>PQ_10</t>
+  </si>
+  <si>
     <t>PQ 2</t>
   </si>
   <si>
-    <t>PQ_1</t>
-  </si>
-  <si>
     <t>PQ 3</t>
   </si>
   <si>
-    <t>PQ_2</t>
-  </si>
-  <si>
     <t>PQ 4</t>
   </si>
   <si>
-    <t>PQ_3</t>
-  </si>
-  <si>
     <t>PQ 5</t>
   </si>
   <si>
-    <t>PQ_4</t>
-  </si>
-  <si>
     <t>PQ 6</t>
   </si>
   <si>
-    <t>PQ_5</t>
-  </si>
-  <si>
     <t>PQ 9</t>
   </si>
   <si>
-    <t>PQ_6</t>
-  </si>
-  <si>
     <t>PQ 10</t>
   </si>
   <si>
-    <t>PQ_7</t>
-  </si>
-  <si>
     <t>PQ 11</t>
   </si>
   <si>
-    <t>PQ_8</t>
-  </si>
-  <si>
     <t>PQ 12</t>
   </si>
   <si>
-    <t>PQ_9</t>
-  </si>
-  <si>
     <t>PQ 13</t>
   </si>
   <si>
-    <t>PQ_10</t>
-  </si>
-  <si>
     <t>PQ 14</t>
   </si>
   <si>
@@ -283,120 +284,120 @@
     <t>Line_0</t>
   </si>
   <si>
+    <t>Line_1</t>
+  </si>
+  <si>
+    <t>Line_2</t>
+  </si>
+  <si>
+    <t>Line_3</t>
+  </si>
+  <si>
+    <t>Line_4</t>
+  </si>
+  <si>
+    <t>Line_5</t>
+  </si>
+  <si>
+    <t>Line_6</t>
+  </si>
+  <si>
+    <t>Line_7</t>
+  </si>
+  <si>
+    <t>Line_8</t>
+  </si>
+  <si>
+    <t>Line_9</t>
+  </si>
+  <si>
+    <t>Line_10</t>
+  </si>
+  <si>
+    <t>Line_11</t>
+  </si>
+  <si>
+    <t>Line_12</t>
+  </si>
+  <si>
+    <t>Line_13</t>
+  </si>
+  <si>
+    <t>Line_14</t>
+  </si>
+  <si>
+    <t>Line_15</t>
+  </si>
+  <si>
+    <t>Line_16</t>
+  </si>
+  <si>
+    <t>Line_17</t>
+  </si>
+  <si>
+    <t>Line_18</t>
+  </si>
+  <si>
+    <t>Line_19</t>
+  </si>
+  <si>
     <t>Line 1-2</t>
   </si>
   <si>
-    <t>Line_1</t>
-  </si>
-  <si>
     <t>Line 1-5</t>
   </si>
   <si>
-    <t>Line_2</t>
-  </si>
-  <si>
     <t>Line 2-3</t>
   </si>
   <si>
-    <t>Line_3</t>
-  </si>
-  <si>
     <t>Line 2-4</t>
   </si>
   <si>
-    <t>Line_4</t>
-  </si>
-  <si>
     <t>Line 2-5</t>
   </si>
   <si>
-    <t>Line_5</t>
-  </si>
-  <si>
     <t>Line 3-4</t>
   </si>
   <si>
-    <t>Line_6</t>
-  </si>
-  <si>
     <t>Line 4-5</t>
   </si>
   <si>
-    <t>Line_7</t>
-  </si>
-  <si>
     <t>Line 4-7</t>
   </si>
   <si>
-    <t>Line_8</t>
-  </si>
-  <si>
     <t>Line 4-9</t>
   </si>
   <si>
-    <t>Line_9</t>
-  </si>
-  <si>
     <t>Line 5-6</t>
   </si>
   <si>
-    <t>Line_10</t>
-  </si>
-  <si>
     <t>Line 6-11</t>
   </si>
   <si>
-    <t>Line_11</t>
-  </si>
-  <si>
     <t>Line 6-12</t>
   </si>
   <si>
-    <t>Line_12</t>
-  </si>
-  <si>
     <t>Line 6-13</t>
   </si>
   <si>
-    <t>Line_13</t>
-  </si>
-  <si>
     <t>Line 7-8</t>
   </si>
   <si>
-    <t>Line_14</t>
-  </si>
-  <si>
     <t>Line 7-9</t>
   </si>
   <si>
-    <t>Line_15</t>
-  </si>
-  <si>
     <t>Line 9-10</t>
   </si>
   <si>
-    <t>Line_16</t>
-  </si>
-  <si>
     <t>Line 9-14</t>
   </si>
   <si>
-    <t>Line_17</t>
-  </si>
-  <si>
     <t>Line 10-11</t>
   </si>
   <si>
-    <t>Line_18</t>
-  </si>
-  <si>
     <t>Line 12-13</t>
   </si>
   <si>
-    <t>Line_19</t>
-  </si>
-  <si>
     <t>Line 13-14</t>
   </si>
   <si>
@@ -430,145 +431,46 @@
     <t>S12</t>
   </si>
   <si>
-    <t>xd</t>
-  </si>
-  <si>
-    <t>xd1</t>
-  </si>
-  <si>
-    <t>xd2</t>
-  </si>
-  <si>
-    <t>xq1</t>
-  </si>
-  <si>
-    <t>xq2</t>
-  </si>
-  <si>
-    <t>Td10</t>
-  </si>
-  <si>
-    <t>Td20</t>
-  </si>
-  <si>
-    <t>Tq10</t>
-  </si>
-  <si>
-    <t>Tq20</t>
-  </si>
-  <si>
-    <t>syn</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>wref0</t>
-  </si>
-  <si>
-    <t>dbl</t>
-  </si>
-  <si>
-    <t>dbu</t>
-  </si>
-  <si>
-    <t>dbc</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t>VMAX</t>
-  </si>
-  <si>
-    <t>VMIN</t>
-  </si>
-  <si>
-    <t>T3</t>
-  </si>
-  <si>
-    <t>Dt</t>
-  </si>
-  <si>
-    <t>TR</t>
-  </si>
-  <si>
-    <t>TA</t>
-  </si>
-  <si>
-    <t>TC</t>
-  </si>
-  <si>
-    <t>TB</t>
-  </si>
-  <si>
-    <t>TE</t>
-  </si>
-  <si>
-    <t>TF1</t>
-  </si>
-  <si>
-    <t>KF1</t>
-  </si>
-  <si>
-    <t>KA</t>
-  </si>
-  <si>
-    <t>KE</t>
-  </si>
-  <si>
-    <t>VRMAX</t>
-  </si>
-  <si>
-    <t>VRMIN</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>SE1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
-    <t>SE2</t>
-  </si>
-  <si>
-    <t>Ae</t>
-  </si>
-  <si>
-    <t>Be</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>dev</t>
-  </si>
-  <si>
-    <t>t</t>
+    <t>GENCLS_1</t>
+  </si>
+  <si>
+    <t>GENCLS_2</t>
+  </si>
+  <si>
+    <t>GENCLS_3</t>
+  </si>
+  <si>
+    <t>GENCLS_4</t>
+  </si>
+  <si>
+    <t>GENCLS_5</t>
+  </si>
+  <si>
+    <t>tf</t>
+  </si>
+  <si>
+    <t>tc</t>
+  </si>
+  <si>
+    <t>xf</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>Fault_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-  </numFmts>
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -576,356 +478,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -948,251 +513,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1200,61 +523,17 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1303,7 +582,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1335,9 +614,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1369,6 +666,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1539,67 +854,66 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1640,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1663,10 +977,10 @@
         <v>0.94</v>
       </c>
       <c r="H3">
-        <v>1.045</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="I3">
-        <v>-0.0869173967493161</v>
+        <v>-8.6917396749316103E-2</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1681,7 +995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1707,7 +1021,7 @@
         <v>1.01</v>
       </c>
       <c r="I4">
-        <v>-0.222005880853675</v>
+        <v>-0.22200588085367501</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1722,7 +1036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1745,10 +1059,10 @@
         <v>0.94</v>
       </c>
       <c r="H5">
-        <v>1.019</v>
+        <v>1.0189999999999999</v>
       </c>
       <c r="I5">
-        <v>-0.180292511731011</v>
+        <v>-0.18029251173101099</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1763,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1789,7 +1103,7 @@
         <v>1.02</v>
       </c>
       <c r="I6">
-        <v>-0.1532399083251</v>
+        <v>-0.15323990832510001</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1804,7 +1118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1830,7 +1144,7 @@
         <v>1.07</v>
       </c>
       <c r="I7">
-        <v>-0.248185819633589</v>
+        <v>-0.24818581963358899</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1845,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1868,7 +1182,7 @@
         <v>0.94</v>
       </c>
       <c r="H8">
-        <v>1.062</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="I8">
         <v>-0.233350520991638</v>
@@ -1886,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1909,10 +1223,10 @@
         <v>0.94</v>
       </c>
       <c r="H9">
-        <v>1.09</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I9">
-        <v>-0.233175988066438</v>
+        <v>-0.23317598806643799</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1927,7 +1241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1953,7 +1267,7 @@
         <v>1.056</v>
       </c>
       <c r="I10">
-        <v>-0.260752190247948</v>
+        <v>-0.26075219024794799</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1968,7 +1282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1991,10 +1305,10 @@
         <v>0.94</v>
       </c>
       <c r="H11">
-        <v>1.051</v>
+        <v>1.0509999999999999</v>
       </c>
       <c r="I11">
-        <v>-0.263544717051139</v>
+        <v>-0.26354471705113902</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -2009,7 +1323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2032,10 +1346,10 @@
         <v>0.94</v>
       </c>
       <c r="H12">
-        <v>1.057</v>
+        <v>1.0569999999999999</v>
       </c>
       <c r="I12">
-        <v>-0.258134196369957</v>
+        <v>-0.25813419636995699</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -2050,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2073,10 +1387,10 @@
         <v>0.94</v>
       </c>
       <c r="H13">
-        <v>1.055</v>
+        <v>1.0549999999999999</v>
       </c>
       <c r="I13">
-        <v>-0.263021118275541</v>
+        <v>-0.26302111827554098</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -2091,7 +1405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2132,7 +1446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2158,7 +1472,7 @@
         <v>1.036</v>
       </c>
       <c r="I15">
-        <v>-0.279950812019886</v>
+        <v>-0.27995081201988598</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2175,293 +1489,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:V1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>171</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>29</v>
@@ -2470,16 +1529,16 @@
         <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2490,7 +1549,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2505,24 +1564,24 @@
         <v>0.127</v>
       </c>
       <c r="I2">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -2531,30 +1590,30 @@
         <v>110</v>
       </c>
       <c r="G3">
-        <v>0.942</v>
+        <v>0.94199999999999995</v>
       </c>
       <c r="H3">
         <v>0.19</v>
       </c>
       <c r="I3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J3">
         <v>0.9</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -2563,30 +1622,30 @@
         <v>110</v>
       </c>
       <c r="G4">
-        <v>0.478</v>
+        <v>0.47799999999999998</v>
       </c>
       <c r="H4">
-        <v>-0.039</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="I4">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J4">
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>5</v>
@@ -2595,30 +1654,30 @@
         <v>110</v>
       </c>
       <c r="G5">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="H5">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="I5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J5">
         <v>0.9</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -2630,27 +1689,27 @@
         <v>0.112</v>
       </c>
       <c r="H6">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I6">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J6">
         <v>0.9</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E7">
         <v>9</v>
@@ -2659,30 +1718,30 @@
         <v>110</v>
       </c>
       <c r="G7">
-        <v>0.295</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="H7">
-        <v>0.166</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="I7">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J7">
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>10</v>
@@ -2694,27 +1753,27 @@
         <v>0.09</v>
       </c>
       <c r="H8">
-        <v>0.058</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="I8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J8">
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>11</v>
@@ -2723,30 +1782,30 @@
         <v>110</v>
       </c>
       <c r="G9">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="H9">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="I9">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J9">
         <v>0.9</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E10">
         <v>12</v>
@@ -2755,30 +1814,30 @@
         <v>110</v>
       </c>
       <c r="G10">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="H10">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="I10">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J10">
         <v>0.9</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E11">
         <v>13</v>
@@ -2787,24 +1846,24 @@
         <v>110</v>
       </c>
       <c r="G11">
-        <v>0.135</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="H11">
-        <v>0.058</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="I11">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J11">
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2819,13 +1878,13 @@
         <v>110</v>
       </c>
       <c r="G12">
-        <v>0.149</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="H12">
         <v>0.05</v>
       </c>
       <c r="I12">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J12">
         <v>0.9</v>
@@ -2833,41 +1892,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -2894,13 +1950,13 @@
         <v>58</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>59</v>
@@ -2909,7 +1965,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2938,7 +1994,7 @@
         <v>0.4</v>
       </c>
       <c r="J2">
-        <v>0.424</v>
+        <v>0.42399999999999999</v>
       </c>
       <c r="K2">
         <v>1.4</v>
@@ -2953,7 +2009,7 @@
         <v>-0.4</v>
       </c>
       <c r="O2">
-        <v>1.045</v>
+        <v>1.0449999999999999</v>
       </c>
       <c r="P2">
         <v>1.4</v>
@@ -2968,7 +2024,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2997,7 +2053,7 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0.234</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -3027,7 +2083,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3086,7 +2142,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3115,7 +2171,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0.174</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -3130,7 +2186,7 @@
         <v>-0.06</v>
       </c>
       <c r="O5">
-        <v>1.09</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="P5">
         <v>1.4</v>
@@ -3147,41 +2203,38 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -3208,13 +2261,13 @@
         <v>58</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>59</v>
@@ -3223,10 +2276,10 @@
         <v>60</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3252,13 +2305,13 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>2.324</v>
+        <v>2.3239999999999998</v>
       </c>
       <c r="J2">
-        <v>-0.169</v>
+        <v>-0.16900000000000001</v>
       </c>
       <c r="K2">
-        <v>3.324</v>
+        <v>3.3239999999999998</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -3290,35 +2343,32 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>28</v>
@@ -3327,7 +2377,7 @@
         <v>53</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>66</v>
@@ -3339,7 +2389,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3373,35 +2423,32 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>71</v>
@@ -3455,16 +2502,16 @@
         <v>83</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3475,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3496,13 +2543,13 @@
         <v>110</v>
       </c>
       <c r="K2">
-        <v>0.01938</v>
+        <v>1.9380000000000001E-2</v>
       </c>
       <c r="L2">
-        <v>0.05917</v>
+        <v>5.917E-2</v>
       </c>
       <c r="M2">
-        <v>0.0528</v>
+        <v>5.28E-2</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -3529,18 +2576,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3561,13 +2608,13 @@
         <v>110</v>
       </c>
       <c r="K3">
-        <v>0.05403</v>
+        <v>5.4030000000000002E-2</v>
       </c>
       <c r="L3">
-        <v>0.22304</v>
+        <v>0.22303999999999999</v>
       </c>
       <c r="M3">
-        <v>0.0492</v>
+        <v>4.9200000000000001E-2</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -3594,18 +2641,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -3626,13 +2673,13 @@
         <v>110</v>
       </c>
       <c r="K4">
-        <v>0.04699</v>
+        <v>4.6989999999999997E-2</v>
       </c>
       <c r="L4">
-        <v>0.19797</v>
+        <v>0.19797000000000001</v>
       </c>
       <c r="M4">
-        <v>0.0438</v>
+        <v>4.3799999999999999E-2</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -3659,18 +2706,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3691,13 +2738,13 @@
         <v>110</v>
       </c>
       <c r="K5">
-        <v>0.05811</v>
+        <v>5.8110000000000002E-2</v>
       </c>
       <c r="L5">
         <v>0.17632</v>
       </c>
       <c r="M5">
-        <v>0.034</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -3724,18 +2771,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -3756,13 +2803,13 @@
         <v>110</v>
       </c>
       <c r="K6">
-        <v>0.05695</v>
+        <v>5.6950000000000001E-2</v>
       </c>
       <c r="L6">
-        <v>0.17388</v>
+        <v>0.17388000000000001</v>
       </c>
       <c r="M6">
-        <v>0.0346</v>
+        <v>3.4599999999999999E-2</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -3789,18 +2836,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -3821,13 +2868,13 @@
         <v>110</v>
       </c>
       <c r="K7">
-        <v>0.06701</v>
+        <v>6.701E-2</v>
       </c>
       <c r="L7">
-        <v>0.17103</v>
+        <v>0.17102999999999999</v>
       </c>
       <c r="M7">
-        <v>0.0128</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -3854,18 +2901,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -3886,10 +2933,10 @@
         <v>110</v>
       </c>
       <c r="K8">
-        <v>0.01335</v>
+        <v>1.3350000000000001E-2</v>
       </c>
       <c r="L8">
-        <v>0.04211</v>
+        <v>4.2110000000000002E-2</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -3919,18 +2966,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="E9">
         <v>4</v>
@@ -3978,24 +3025,24 @@
         <v>1</v>
       </c>
       <c r="T9">
-        <v>0.978</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="U9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -4019,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0.55618</v>
+        <v>0.55618000000000001</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -4043,24 +3090,24 @@
         <v>1</v>
       </c>
       <c r="T10">
-        <v>0.969</v>
+        <v>0.96899999999999997</v>
       </c>
       <c r="U10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -4084,7 +3131,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>0.25202</v>
+        <v>0.25202000000000002</v>
       </c>
       <c r="M11">
         <v>0</v>
@@ -4108,24 +3155,24 @@
         <v>1</v>
       </c>
       <c r="T11">
-        <v>0.932</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="U11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -4146,10 +3193,10 @@
         <v>110</v>
       </c>
       <c r="K12">
-        <v>0.09498</v>
+        <v>9.4979999999999995E-2</v>
       </c>
       <c r="L12">
-        <v>0.1989</v>
+        <v>0.19889999999999999</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -4179,18 +3226,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E13">
         <v>6</v>
@@ -4211,10 +3258,10 @@
         <v>110</v>
       </c>
       <c r="K13">
-        <v>0.12291</v>
+        <v>0.12291000000000001</v>
       </c>
       <c r="L13">
-        <v>0.25581</v>
+        <v>0.25580999999999998</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -4244,18 +3291,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -4276,7 +3323,7 @@
         <v>110</v>
       </c>
       <c r="K14">
-        <v>0.06615</v>
+        <v>6.615E-2</v>
       </c>
       <c r="L14">
         <v>0.13027</v>
@@ -4309,18 +3356,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E15">
         <v>7</v>
@@ -4374,18 +3421,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E16">
         <v>7</v>
@@ -4439,18 +3486,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E17">
         <v>9</v>
@@ -4471,10 +3518,10 @@
         <v>110</v>
       </c>
       <c r="K17">
-        <v>0.03181</v>
+        <v>3.1809999999999998E-2</v>
       </c>
       <c r="L17">
-        <v>0.0845</v>
+        <v>8.4500000000000006E-2</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -4504,18 +3551,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="E18">
         <v>9</v>
@@ -4539,7 +3586,7 @@
         <v>0.12711</v>
       </c>
       <c r="L18">
-        <v>0.27038</v>
+        <v>0.27038000000000001</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -4569,18 +3616,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E19">
         <v>10</v>
@@ -4601,10 +3648,10 @@
         <v>110</v>
       </c>
       <c r="K19">
-        <v>0.08205</v>
+        <v>8.2049999999999998E-2</v>
       </c>
       <c r="L19">
-        <v>0.19207</v>
+        <v>0.19206999999999999</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -4634,18 +3681,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E20">
         <v>12</v>
@@ -4666,7 +3713,7 @@
         <v>110</v>
       </c>
       <c r="K20">
-        <v>0.22092</v>
+        <v>0.22092000000000001</v>
       </c>
       <c r="L20">
         <v>0.19988</v>
@@ -4699,12 +3746,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -4766,222 +3813,428 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>615</v>
+      </c>
+      <c r="I2">
+        <v>69</v>
+      </c>
+      <c r="J2">
+        <v>60</v>
+      </c>
+      <c r="K2">
+        <v>3.01</v>
+      </c>
+      <c r="L2">
+        <v>6.02</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <v>69</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>3.01</v>
+      </c>
+      <c r="L3">
+        <v>6.02</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+      <c r="I4">
+        <v>69</v>
+      </c>
+      <c r="J4">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>3.01</v>
+      </c>
+      <c r="L4">
+        <v>6.02</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5">
+        <v>13.8</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>3.01</v>
+      </c>
+      <c r="L5">
+        <v>6.02</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>60</v>
+      </c>
+      <c r="K6">
+        <v>3.01</v>
+      </c>
+      <c r="L6">
+        <v>6.02</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:S1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>133</v>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2.02</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AB1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>